<commit_message>
able to parse exceldates with xml keyword exceldate
</commit_message>
<xml_diff>
--- a/src/test/resources/model/input/xlsx2.xlsx
+++ b/src/test/resources/model/input/xlsx2.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>Intheader</t>
   </si>
@@ -29,6 +29,9 @@
   </si>
   <si>
     <t>Floots</t>
+  </si>
+  <si>
+    <t>lelijke_excel_dates</t>
   </si>
   <si>
     <t>row2</t>
@@ -113,8 +116,9 @@
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="42"/>
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="9"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0"/>
     <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="165" xfId="0"/>
   </cellXfs>
   <cellStyles count="6">
@@ -133,16 +137,16 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="A1" activeCellId="0" pane="topLeft" sqref="A1"/>
+      <selection activeCell="F1" activeCellId="0" pane="topLeft" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="11.6313725490196"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="8.67450980392157"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="11.6313725490196"/>
+    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="11.6941176470588"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="8.71764705882353"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="11.6941176470588"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="1">
@@ -158,19 +162,25 @@
       <c r="D1" s="0" t="s">
         <v>3</v>
       </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="2">
       <c r="A2" s="0" t="n">
         <v>1</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="C2" s="2" t="n">
         <v>34950.3813541667</v>
       </c>
       <c r="D2" s="0" t="n">
         <v>0.8</v>
+      </c>
+      <c r="E2" s="1" t="n">
+        <v>41080</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="3">
@@ -178,22 +188,26 @@
         <v>8</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>5</v>
-      </c>
-      <c r="C3" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="C3" s="2" t="n">
         <v>35042.5508449074</v>
       </c>
       <c r="D3" s="0" t="n">
         <v>13.13</v>
       </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="4">
+      <c r="E3" s="1"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.65" outlineLevel="0" r="4">
       <c r="B4" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="C4" s="1"/>
+        <v>7</v>
+      </c>
+      <c r="C4" s="2"/>
       <c r="D4" s="0" t="n">
         <v>21.21</v>
+      </c>
+      <c r="E4" s="1" t="n">
+        <v>41081</v>
       </c>
     </row>
   </sheetData>
@@ -219,7 +233,7 @@
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.6313725490196"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.6941176470588"/>
   </cols>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -244,7 +258,7 @@
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.6313725490196"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.6941176470588"/>
   </cols>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
Add NULL string cells to parser
</commit_message>
<xml_diff>
--- a/src/test/resources/model/input/xlsx2.xlsx
+++ b/src/test/resources/model/input/xlsx2.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>Intheader</t>
   </si>
@@ -41,6 +41,9 @@
   </si>
   <si>
     <t>dingen</t>
+  </si>
+  <si>
+    <t>NULL</t>
   </si>
 </sst>
 </file>
@@ -140,13 +143,13 @@
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="F1" activeCellId="0" pane="topLeft" sqref="F1"/>
+      <selection activeCell="C1" activeCellId="0" pane="topLeft" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="11.6941176470588"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="8.71764705882353"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="11.6941176470588"/>
+    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="11.7490196078431"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="8.76470588235294"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="11.7490196078431"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="1">
@@ -202,7 +205,9 @@
       <c r="B4" s="0" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="2"/>
+      <c r="C4" s="2" t="s">
+        <v>8</v>
+      </c>
       <c r="D4" s="0" t="n">
         <v>21.21</v>
       </c>
@@ -233,7 +238,7 @@
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.6941176470588"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.7490196078431"/>
   </cols>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -258,7 +263,7 @@
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.6941176470588"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.7490196078431"/>
   </cols>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
add boolvalue to parser
</commit_message>
<xml_diff>
--- a/src/test/resources/model/input/xlsx2.xlsx
+++ b/src/test/resources/model/input/xlsx2.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>Intheader</t>
   </si>
@@ -32,6 +32,9 @@
   </si>
   <si>
     <t>lelijke_excel_dates</t>
+  </si>
+  <si>
+    <t>Booleans</t>
   </si>
   <si>
     <t>row2</t>
@@ -50,9 +53,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt formatCode="GENERAL" numFmtId="164"/>
     <numFmt formatCode="DD/MM/YY" numFmtId="165"/>
+    <numFmt formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;" numFmtId="166"/>
   </numFmts>
   <fonts count="4">
     <font>
@@ -119,10 +123,11 @@
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="42"/>
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="9"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0"/>
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0"/>
     <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="165" xfId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="166" xfId="0"/>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle builtinId="0" customBuiltin="false" name="Normal" xfId="0"/>
@@ -140,16 +145,18 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="C1" activeCellId="0" pane="topLeft" sqref="C1"/>
+      <selection activeCell="F4" activeCellId="0" pane="topLeft" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="11.7490196078431"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="8.76470588235294"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="11.7490196078431"/>
+    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="11.8117647058824"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="8.8078431372549"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="11.8117647058824"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="17.1764705882353"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="11.8117647058824"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="1">
@@ -168,13 +175,16 @@
       <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
+      <c r="F1" s="0" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="2">
       <c r="A2" s="0" t="n">
         <v>1</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C2" s="2" t="n">
         <v>34950.3813541667</v>
@@ -184,6 +194,9 @@
       </c>
       <c r="E2" s="1" t="n">
         <v>41080</v>
+      </c>
+      <c r="F2" s="3" t="b">
+        <v>1</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="3">
@@ -191,7 +204,7 @@
         <v>8</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C3" s="2" t="n">
         <v>35042.5508449074</v>
@@ -200,13 +213,16 @@
         <v>13.13</v>
       </c>
       <c r="E3" s="1"/>
+      <c r="F3" s="3" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.65" outlineLevel="0" r="4">
       <c r="B4" s="0" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D4" s="0" t="n">
         <v>21.21</v>
@@ -238,7 +254,7 @@
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.7490196078431"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.8117647058824"/>
   </cols>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -263,7 +279,7 @@
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.7490196078431"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.8117647058824"/>
   </cols>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>